<commit_message>
Commit inicial (Base de dados e análise)
</commit_message>
<xml_diff>
--- a/QUESTIONÁRIO SOBRE O CONSUMO DE ÁLCOOL ENTRE OS ESTUDANTES DA UEFS (respostas).xlsx
+++ b/QUESTIONÁRIO SOBRE O CONSUMO DE ÁLCOOL ENTRE OS ESTUDANTES DA UEFS (respostas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="81">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>1 a 2 copos por dia</t>
+  </si>
+  <si>
+    <t>A partir do 10º semestre</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Y58" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Y72" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="25">
     <tableColumn name="Carimbo de data/hora" id="1"/>
     <tableColumn name="Sexo" id="2"/>
@@ -5219,79 +5222,1157 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="16">
+      <c r="A58" s="13">
         <v>45836.58988435185</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E58" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F58" s="17" t="s">
+      <c r="E58" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G58" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H58" s="17" t="s">
+      <c r="G58" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H58" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I58" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="J58" s="17" t="s">
+      <c r="J58" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="L58" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="N58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="O58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="P58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="R58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="S58" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="T58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="U58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="V58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="W58" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="X58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y58" s="18" t="s">
+      <c r="K58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L58" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S58" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W58" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="X58" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y58" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10">
+        <v>45836.60610662037</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L59" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S59" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X59" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y59" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="13">
+        <v>45836.60891416667</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J60" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L60" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W60" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X60" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y60" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="10">
+        <v>45836.66388969908</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J61" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S61" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W61" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X61" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y61" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="13">
+        <v>45836.6666487037</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I62" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J62" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L62" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X62" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y62" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="10">
+        <v>45836.66759834491</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N63" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O63" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P63" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q63" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R63" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S63" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T63" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U63" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V63" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y63" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="13">
+        <v>45836.66823284722</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I64" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J64" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W64" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="X64" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y64" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="10">
+        <v>45836.6792771412</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L65" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X65" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y65" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="13">
+        <v>45836.6795049537</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J66" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L66" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N66" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O66" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P66" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q66" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R66" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S66" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W66" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="X66" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y66" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="10">
+        <v>45836.67991284722</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J67" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K67" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N67" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P67" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q67" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="R67" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S67" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T67" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U67" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V67" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y67" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="13">
+        <v>45836.75218818287</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N68" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="O68" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="P68" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q68" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="R68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S68" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="T68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="U68" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="W68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="X68" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y68" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="10">
+        <v>45836.753425648145</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J69" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L69" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M69" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N69" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O69" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P69" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q69" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R69" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S69" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W69" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y69" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="13">
+        <v>45836.80481577547</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M70" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N70" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O70" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P70" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q70" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="R70" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S70" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X70" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y70" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="10">
+        <v>45836.8887953588</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N71" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O71" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P71" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q71" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="R71" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S71" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T71" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U71" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="W71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X71" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y71" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="16">
+        <v>45836.95655461805</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J72" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="O72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="S72" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="T72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="U72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="V72" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="W72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="X72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y72" s="18" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>